<commit_message>
Updated based on definition and tooling fixes
</commit_message>
<xml_diff>
--- a/docs/oncocore-CancerGeneticMarkerAnalysisResult.xlsx
+++ b/docs/oncocore-CancerGeneticMarkerAnalysisResult.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2672" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="428">
   <si>
     <t>Path</t>
   </si>
@@ -469,14 +469,7 @@
     <t>Observation.extension.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
+    <t>Extension.id</t>
   </si>
   <si>
     <t>Observation.extension.extension</t>
@@ -488,7 +481,7 @@
     <t>An Extension</t>
   </si>
   <si>
-    <t>Element.extension</t>
+    <t>Extension.extension</t>
   </si>
   <si>
     <t>Observation.extension.url</t>
@@ -500,7 +493,10 @@
     <t>Source of the definition for the extension code - a logical name or a URL.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://hl7.org/fhir/us/fhirURL/StructureDefinition/oncocore-GeneName-extension"/&gt;</t>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition should be version specific.  This will ideally be the URI for the Resource Profile defining the extension, with the code for the extension after a #.</t>
+  </si>
+  <si>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://hl7.org/fhir/StructureDefinition/geneticsGene"/&gt;</t>
   </si>
   <si>
     <t>Extension.url</t>
@@ -888,6 +884,10 @@
   </si>
   <si>
     <t>Observation.comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string {[]} {[]}
+</t>
   </si>
   <si>
     <t>Comments about result</t>
@@ -3701,13 +3701,13 @@
         <v>42</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>144</v>
+        <v>53</v>
       </c>
       <c r="K21" t="s" s="2">
         <v>62</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3758,7 +3758,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3776,7 +3776,7 @@
         <v>42</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>42</v>
@@ -3784,7 +3784,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3810,10 +3810,10 @@
         <v>67</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3864,7 +3864,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3916,61 +3916,63 @@
         <v>81</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="L23" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>42</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="R23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE23" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="R23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="S23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="T23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="U23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="V23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="W23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Y23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Z23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE23" t="s" s="2">
-        <v>155</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>51</v>
@@ -3996,7 +3998,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4019,13 +4021,13 @@
         <v>42</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>157</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>158</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>159</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -4056,25 +4058,25 @@
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="Z24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD24" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE24" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="Z24" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA24" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB24" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC24" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD24" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE24" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -4103,7 +4105,7 @@
         <v>126</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>42</v>
@@ -4125,11 +4127,11 @@
         <v>42</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4209,7 +4211,7 @@
         <v>126</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>42</v>
@@ -4231,11 +4233,11 @@
         <v>42</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" t="s" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4315,7 +4317,7 @@
         <v>126</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>42</v>
@@ -4337,11 +4339,11 @@
         <v>42</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" t="s" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4418,7 +4420,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4444,10 +4446,10 @@
         <v>67</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>172</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>173</v>
       </c>
       <c r="M28" t="s" s="2">
         <v>70</v>
@@ -4500,7 +4502,7 @@
         <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
@@ -4526,7 +4528,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4549,17 +4551,17 @@
         <v>42</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>42</v>
@@ -4608,7 +4610,7 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4623,18 +4625,18 @@
         <v>42</v>
       </c>
       <c r="AJ29" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AK29" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="AK29" t="s" s="2">
-        <v>180</v>
-      </c>
       <c r="AL29" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4660,14 +4662,14 @@
         <v>104</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>182</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>183</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>42</v>
@@ -4696,51 +4698,51 @@
       </c>
       <c r="X30" s="2"/>
       <c r="Y30" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE30" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="Z30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI30" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ30" t="s" s="2">
+      <c r="AK30" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="AK30" t="s" s="2">
+      <c r="AL30" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="AL30" t="s" s="2">
-        <v>188</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4763,16 +4765,16 @@
         <v>42</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4783,7 +4785,7 @@
         <v>42</v>
       </c>
       <c r="R31" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S31" t="s" s="2">
         <v>42</v>
@@ -4801,58 +4803,58 @@
         <v>97</v>
       </c>
       <c r="X31" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="Y31" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="Y31" t="s" s="2">
+      <c r="Z31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE31" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="Z31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AK31" t="s" s="2">
+      <c r="AL31" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>197</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -4871,19 +4873,19 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="M32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>203</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>42</v>
@@ -4912,51 +4914,51 @@
       </c>
       <c r="X32" s="2"/>
       <c r="Y32" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE32" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="Z32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="AF32" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
+      <c r="AK32" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="AK32" t="s" s="2">
+      <c r="AL32" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4979,19 +4981,19 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="K33" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="K33" t="s" s="2">
+      <c r="L33" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="M33" t="s" s="2">
+      <c r="N33" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>42</v>
@@ -5040,7 +5042,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5055,18 +5057,18 @@
         <v>42</v>
       </c>
       <c r="AJ33" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AK33" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="AK33" t="s" s="2">
+      <c r="AL33" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>216</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5089,17 +5091,17 @@
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>42</v>
@@ -5148,7 +5150,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -5163,18 +5165,18 @@
         <v>42</v>
       </c>
       <c r="AJ34" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AK34" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="AK34" t="s" s="2">
+      <c r="AL34" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AL34" t="s" s="2">
-        <v>224</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5197,19 +5199,19 @@
         <v>42</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>42</v>
@@ -5258,7 +5260,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -5270,21 +5272,21 @@
         <v>42</v>
       </c>
       <c r="AI35" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="AJ35" t="s" s="2">
+      <c r="AK35" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="AK35" t="s" s="2">
+      <c r="AL35" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>234</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5310,13 +5312,13 @@
         <v>76</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5366,7 +5368,7 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5381,18 +5383,18 @@
         <v>42</v>
       </c>
       <c r="AJ36" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="AK36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AL36" t="s" s="2">
-        <v>241</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5415,17 +5417,17 @@
         <v>52</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K37" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="K37" t="s" s="2">
+      <c r="L37" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>42</v>
@@ -5474,7 +5476,7 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5489,18 +5491,18 @@
         <v>42</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AK37" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="AK37" t="s" s="2">
+      <c r="AL37" t="s" s="2">
         <v>248</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>249</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5523,19 +5525,19 @@
         <v>42</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="K38" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="K38" t="s" s="2">
+      <c r="L38" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>42</v>
@@ -5584,7 +5586,7 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5596,13 +5598,13 @@
         <v>42</v>
       </c>
       <c r="AI38" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="AJ38" t="s" s="2">
+      <c r="AK38" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>42</v>
@@ -5610,7 +5612,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5633,19 +5635,19 @@
         <v>42</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>262</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>263</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>42</v>
@@ -5674,34 +5676,34 @@
       </c>
       <c r="X39" s="2"/>
       <c r="Y39" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="Z39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE39" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH39" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="AF39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>265</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>42</v>
@@ -5710,7 +5712,7 @@
         <v>125</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>42</v>
@@ -5718,11 +5720,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5741,17 +5743,17 @@
         <v>42</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>42</v>
@@ -5779,46 +5781,46 @@
         <v>90</v>
       </c>
       <c r="X40" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="Y40" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="Y40" t="s" s="2">
+      <c r="Z40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
         <v>273</v>
       </c>
-      <c r="Z40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
+      <c r="AK40" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>42</v>
@@ -5826,7 +5828,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5849,7 +5851,7 @@
         <v>42</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="K41" t="s" s="2">
         <v>277</v>
@@ -5908,7 +5910,7 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5957,7 +5959,7 @@
         <v>42</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K42" t="s" s="2">
         <v>283</v>
@@ -6377,7 +6379,7 @@
         <v>52</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="K46" t="s" s="2">
         <v>301</v>
@@ -6483,7 +6485,7 @@
         <v>42</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>308</v>
@@ -7134,7 +7136,7 @@
         <v>67</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>342</v>
@@ -7451,7 +7453,7 @@
         <v>42</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K56" t="s" s="2">
         <v>355</v>
@@ -7530,7 +7532,7 @@
         <v>361</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>42</v>
@@ -7669,7 +7671,7 @@
         <v>42</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="K58" t="s" s="2">
         <v>369</v>
@@ -8102,7 +8104,7 @@
         <v>67</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L62" t="s" s="2">
         <v>342</v>
@@ -8750,7 +8752,7 @@
         <v>67</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L68" t="s" s="2">
         <v>342</v>
@@ -8855,7 +8857,7 @@
         <v>52</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K69" t="s" s="2">
         <v>406</v>
@@ -8865,7 +8867,7 @@
       </c>
       <c r="M69" s="2"/>
       <c r="N69" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -8929,13 +8931,13 @@
         <v>42</v>
       </c>
       <c r="AJ69" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AK69" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="AK69" t="s" s="2">
+      <c r="AL69" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>207</v>
       </c>
     </row>
     <row r="70" hidden="true">
@@ -8963,7 +8965,7 @@
         <v>52</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K70" t="s" s="2">
         <v>412</v>
@@ -8975,7 +8977,7 @@
         <v>414</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>42</v>
@@ -9039,10 +9041,10 @@
         <v>42</v>
       </c>
       <c r="AJ70" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="AK70" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>42</v>
@@ -9073,19 +9075,19 @@
         <v>42</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K71" t="s" s="2">
         <v>416</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M71" t="s" s="2">
         <v>417</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>42</v>
@@ -9114,7 +9116,7 @@
       </c>
       <c r="X71" s="2"/>
       <c r="Y71" t="s" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z71" t="s" s="2">
         <v>42</v>
@@ -9141,7 +9143,7 @@
         <v>51</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>42</v>
@@ -9150,7 +9152,7 @@
         <v>125</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>42</v>
@@ -9500,7 +9502,7 @@
         <v>67</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L75" t="s" s="2">
         <v>342</v>
@@ -9805,7 +9807,7 @@
         <v>42</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K78" t="s" s="2">
         <v>355</v>
@@ -9880,7 +9882,7 @@
         <v>361</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>42</v>
@@ -10015,7 +10017,7 @@
         <v>42</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>144</v>
+        <v>276</v>
       </c>
       <c r="K80" t="s" s="2">
         <v>369</v>

</xml_diff>

<commit_message>
Update to mCODE 0.7
</commit_message>
<xml_diff>
--- a/docs/oncocore-CancerGeneticMarkerAnalysisResult.xlsx
+++ b/docs/oncocore-CancerGeneticMarkerAnalysisResult.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$79</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="425">
   <si>
     <t>Path</t>
   </si>
@@ -539,16 +539,6 @@
   </si>
   <si>
     <t>A DNA Marker identifier conveys a universal or standard repository identifier for definitive characterstics of a DNA Marker. (recommend using NCBI dbSNP ids - rs#) (source: LOINC)</t>
-  </si>
-  <si>
-    <t>recorder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-base-Recorder-extension]]} {[]}
-</t>
-  </si>
-  <si>
-    <t>The recorder of the information, if other than the information originator. For example, the nurse taking a list of medications reported by the patient.</t>
   </si>
   <si>
     <t>Observation.modifierExtension</t>
@@ -673,7 +663,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-Patient]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Patient]]}
 </t>
   </si>
   <si>
@@ -701,7 +691,7 @@
     <t>Observation.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-encounter-Encounter]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Encounter]]}
 </t>
   </si>
   <si>
@@ -779,7 +769,7 @@
     <t>Observation.performer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-Practitioner], CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-Organization], CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-Patient], CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-RelatedPerson]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Practitioner], CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Organization], CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Patient], CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-RelatedPerson]]}
 </t>
   </si>
   <si>
@@ -1007,7 +997,7 @@
     <t>Observation.specimen</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-Specimen]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Specimen]]}
 </t>
   </si>
   <si>
@@ -1029,7 +1019,7 @@
     <t>Observation.device</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-entity-Device]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Device]]}
 </t>
   </si>
   <si>
@@ -1243,7 +1233,7 @@
     <t>Observation.related.target</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/fhirURL/StructureDefinition/shr-base-Observation]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/shr/StructureDefinition/shr-core-Observation]]}
 </t>
   </si>
   <si>
@@ -1499,7 +1489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM80"/>
+  <dimension ref="A1:AM79"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1508,44 +1498,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="53.546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="31.46484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="54.46484375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="31.7109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.5546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="94.64453125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="70.21484375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="42.92578125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="95.21875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="70.0234375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="43.6015625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="128.71484375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="102.734375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="22.0078125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="124.46875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="103.87890625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="22.03125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4314,38 +4304,40 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="B27" t="s" s="2">
         <v>167</v>
       </c>
+      <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="K27" s="2"/>
       <c r="L27" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="M27" s="2"/>
+      <c r="M27" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>42</v>
@@ -4394,7 +4386,7 @@
         <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -4412,7 +4404,7 @@
         <v>42</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>42</v>
@@ -4424,7 +4416,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4437,24 +4429,24 @@
         <v>42</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="N28" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" t="s" s="2">
+        <v>174</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>42</v>
       </c>
@@ -4517,18 +4509,18 @@
         <v>42</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>42</v>
+        <v>175</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>42</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4536,32 +4528,32 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>174</v>
+        <v>104</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" t="s" s="2">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>42</v>
@@ -4586,13 +4578,11 @@
         <v>40</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X29" t="s" s="2">
-        <v>42</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="X29" s="2"/>
       <c r="Y29" t="s" s="2">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>42</v>
@@ -4610,13 +4600,13 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>42</v>
@@ -4625,18 +4615,18 @@
         <v>42</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4653,24 +4643,24 @@
         <v>52</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" t="s" s="2">
-        <v>183</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>42</v>
       </c>
@@ -4679,7 +4669,7 @@
         <v>42</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>42</v>
@@ -4694,11 +4684,13 @@
         <v>40</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="X30" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="Y30" t="s" s="2">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>42</v>
@@ -4716,10 +4708,10 @@
         <v>42</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>51</v>
@@ -4731,22 +4723,22 @@
         <v>42</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>185</v>
+        <v>42</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>42</v>
+        <v>195</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4768,15 +4760,17 @@
         <v>156</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="N31" s="2"/>
+        <v>198</v>
+      </c>
+      <c r="N31" t="s" s="2">
+        <v>199</v>
+      </c>
       <c r="O31" t="s" s="2">
         <v>42</v>
       </c>
@@ -4785,7 +4779,7 @@
         <v>42</v>
       </c>
       <c r="R31" t="s" s="2">
-        <v>192</v>
+        <v>42</v>
       </c>
       <c r="S31" t="s" s="2">
         <v>42</v>
@@ -4800,34 +4794,32 @@
         <v>40</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="X31" t="s" s="2">
-        <v>193</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="X31" s="2"/>
       <c r="Y31" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE31" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="Z31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>188</v>
-      </c>
       <c r="AF31" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>51</v>
@@ -4839,22 +4831,22 @@
         <v>42</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>42</v>
+        <v>201</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>198</v>
+        <v>42</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -4873,19 +4865,19 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>42</v>
@@ -4910,11 +4902,13 @@
         <v>40</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="X32" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="Y32" t="s" s="2">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>42</v>
@@ -4932,10 +4926,10 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>51</v>
@@ -4947,18 +4941,18 @@
         <v>42</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4966,13 +4960,13 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s" s="2">
         <v>51</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>42</v>
@@ -4981,19 +4975,17 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>211</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" t="s" s="2">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>42</v>
@@ -5042,7 +5034,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5057,18 +5049,18 @@
         <v>42</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5082,7 +5074,7 @@
         <v>51</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>42</v>
@@ -5091,17 +5083,19 @@
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="M34" s="2"/>
+        <v>224</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>225</v>
+      </c>
       <c r="N34" t="s" s="2">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>42</v>
@@ -5150,7 +5144,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -5162,21 +5156,21 @@
         <v>42</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>42</v>
+        <v>227</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5190,29 +5184,27 @@
         <v>51</v>
       </c>
       <c r="G35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I35" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="H35" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="I35" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="J35" t="s" s="2">
-        <v>225</v>
+        <v>76</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>229</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>42</v>
       </c>
@@ -5260,7 +5252,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -5272,21 +5264,21 @@
         <v>42</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>230</v>
+        <v>42</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5297,7 +5289,7 @@
         <v>40</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>42</v>
@@ -5309,18 +5301,18 @@
         <v>52</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>76</v>
+        <v>239</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N36" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" t="s" s="2">
+        <v>242</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>42</v>
       </c>
@@ -5368,13 +5360,13 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>42</v>
@@ -5383,18 +5375,18 @@
         <v>42</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5405,29 +5397,31 @@
         <v>40</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>42</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>249</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>250</v>
+      </c>
       <c r="N37" t="s" s="2">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>42</v>
@@ -5476,33 +5470,33 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>42</v>
+        <v>252</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>248</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5513,7 +5507,7 @@
         <v>40</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>52</v>
@@ -5525,19 +5519,19 @@
         <v>42</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>42</v>
@@ -5562,13 +5556,11 @@
         <v>40</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X38" t="s" s="2">
-        <v>42</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="X38" s="2"/>
       <c r="Y38" t="s" s="2">
-        <v>42</v>
+        <v>260</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>42</v>
@@ -5586,7 +5578,7 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5595,28 +5587,28 @@
         <v>51</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>42</v>
+        <v>261</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>255</v>
+        <v>42</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>256</v>
+        <v>125</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5626,7 +5618,7 @@
         <v>51</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>42</v>
@@ -5638,16 +5630,14 @@
         <v>156</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>261</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>42</v>
@@ -5674,27 +5664,29 @@
       <c r="W39" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="X39" s="2"/>
+      <c r="X39" t="s" s="2">
+        <v>268</v>
+      </c>
       <c r="Y39" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="Z39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE39" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>258</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5703,16 +5695,16 @@
         <v>51</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>264</v>
+        <v>42</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>125</v>
+        <v>270</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>42</v>
@@ -5720,11 +5712,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>267</v>
+        <v>42</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5743,17 +5735,17 @@
         <v>42</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>156</v>
+        <v>273</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>42</v>
@@ -5778,31 +5770,31 @@
         <v>40</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>271</v>
+        <v>42</v>
       </c>
       <c r="Y40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE40" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5817,10 +5809,10 @@
         <v>42</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>42</v>
@@ -5828,7 +5820,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5839,7 +5831,7 @@
         <v>40</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>42</v>
@@ -5851,17 +5843,19 @@
         <v>42</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>276</v>
+        <v>156</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="M41" s="2"/>
+        <v>281</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>282</v>
+      </c>
       <c r="N41" t="s" s="2">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>42</v>
@@ -5886,13 +5880,11 @@
         <v>40</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>42</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="X41" s="2"/>
       <c r="Y41" t="s" s="2">
-        <v>42</v>
+        <v>285</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>42</v>
@@ -5910,7 +5902,7 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5925,10 +5917,10 @@
         <v>42</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>42</v>
@@ -5936,7 +5928,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5947,7 +5939,7 @@
         <v>40</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>42</v>
@@ -5959,20 +5951,16 @@
         <v>42</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>156</v>
+        <v>53</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>283</v>
+        <v>62</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>286</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>42</v>
       </c>
@@ -5993,14 +5981,16 @@
         <v>42</v>
       </c>
       <c r="V42" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="X42" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="Y42" t="s" s="2">
-        <v>288</v>
+        <v>42</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>42</v>
@@ -6017,15 +6007,11 @@
       <c r="AD42" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="AE42" t="s" s="2">
-        <v>282</v>
-      </c>
+      <c r="AE42" s="2"/>
       <c r="AF42" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AG42" t="s" s="2">
-        <v>51</v>
-      </c>
+      <c r="AG42" s="2"/>
       <c r="AH42" t="s" s="2">
         <v>42</v>
       </c>
@@ -6033,10 +6019,10 @@
         <v>42</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>289</v>
+        <v>42</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>290</v>
+        <v>64</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>42</v>
@@ -6044,18 +6030,18 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>42</v>
@@ -6067,15 +6053,17 @@
         <v>42</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="M43" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>42</v>
@@ -6146,11 +6134,11 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -6166,21 +6154,23 @@
         <v>42</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>68</v>
+        <v>291</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>69</v>
+        <v>292</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="N44" s="2"/>
+        <v>293</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>294</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>42</v>
       </c>
@@ -6239,10 +6229,10 @@
         <v>42</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>42</v>
+        <v>295</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>64</v>
+        <v>296</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>42</v>
@@ -6250,7 +6240,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6261,7 +6251,7 @@
         <v>40</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>42</v>
@@ -6273,19 +6263,19 @@
         <v>52</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>86</v>
+        <v>273</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>42</v>
@@ -6345,10 +6335,10 @@
         <v>42</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>42</v>
@@ -6356,7 +6346,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6376,22 +6366,22 @@
         <v>42</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>276</v>
+        <v>156</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>42</v>
@@ -6413,16 +6403,14 @@
         <v>42</v>
       </c>
       <c r="V46" t="s" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X46" t="s" s="2">
-        <v>42</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="X46" s="2"/>
       <c r="Y46" t="s" s="2">
-        <v>42</v>
+        <v>309</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>42</v>
@@ -6439,11 +6427,15 @@
       <c r="AD46" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="AE46" s="2"/>
+      <c r="AE46" t="s" s="2">
+        <v>304</v>
+      </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AG46" s="2"/>
+      <c r="AG46" t="s" s="2">
+        <v>51</v>
+      </c>
       <c r="AH46" t="s" s="2">
         <v>42</v>
       </c>
@@ -6451,10 +6443,10 @@
         <v>42</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>42</v>
@@ -6462,7 +6454,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6485,20 +6477,18 @@
         <v>42</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>156</v>
+        <v>313</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>311</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>42</v>
       </c>
@@ -6522,29 +6512,31 @@
         <v>40</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="X47" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="Y47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE47" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="Z47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6559,10 +6551,10 @@
         <v>42</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>42</v>
@@ -6570,7 +6562,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6593,16 +6585,16 @@
         <v>42</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6652,7 +6644,7 @@
         <v>42</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6667,10 +6659,10 @@
         <v>42</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>42</v>
@@ -6678,7 +6670,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6689,7 +6681,7 @@
         <v>40</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>42</v>
@@ -6701,18 +6693,20 @@
         <v>42</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="N49" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>331</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>42</v>
       </c>
@@ -6760,25 +6754,25 @@
         <v>42</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>42</v>
+        <v>332</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>42</v>
@@ -6786,7 +6780,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6797,7 +6791,7 @@
         <v>40</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>42</v>
@@ -6809,20 +6803,16 @@
         <v>42</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>331</v>
+        <v>62</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>334</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>42</v>
       </c>
@@ -6870,25 +6860,25 @@
         <v>42</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>335</v>
+        <v>42</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>336</v>
+        <v>42</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>337</v>
+        <v>64</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>42</v>
@@ -6896,18 +6886,18 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>42</v>
@@ -6919,15 +6909,17 @@
         <v>42</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="M51" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>42</v>
@@ -6976,13 +6968,13 @@
         <v>42</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>42</v>
@@ -7002,11 +6994,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7019,7 +7011,7 @@
         <v>42</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I52" t="s" s="2">
         <v>42</v>
@@ -7028,10 +7020,10 @@
         <v>67</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>69</v>
+        <v>339</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>70</v>
@@ -7084,7 +7076,7 @@
         <v>42</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7102,7 +7094,7 @@
         <v>42</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>42</v>
@@ -7114,36 +7106,34 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>341</v>
+        <v>42</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I53" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>67</v>
+        <v>341</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>171</v>
+        <v>342</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>42</v>
@@ -7198,19 +7188,19 @@
         <v>40</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>42</v>
+        <v>344</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>42</v>
+        <v>345</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>125</v>
+        <v>346</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>42</v>
@@ -7218,7 +7208,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7241,13 +7231,13 @@
         <v>42</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7298,7 +7288,7 @@
         <v>42</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>40</v>
@@ -7307,16 +7297,16 @@
         <v>51</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>42</v>
@@ -7324,7 +7314,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7347,16 +7337,20 @@
         <v>42</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>344</v>
+        <v>156</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>355</v>
+      </c>
       <c r="O55" t="s" s="2">
         <v>42</v>
       </c>
@@ -7380,13 +7374,13 @@
         <v>40</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>42</v>
+        <v>356</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>42</v>
+        <v>357</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>42</v>
@@ -7404,7 +7398,7 @@
         <v>42</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7413,16 +7407,16 @@
         <v>51</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>347</v>
+        <v>42</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>353</v>
+        <v>271</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>42</v>
@@ -7430,7 +7424,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7453,19 +7447,17 @@
         <v>42</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>156</v>
+        <v>360</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>357</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="M56" s="2"/>
       <c r="N56" t="s" s="2">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>42</v>
@@ -7490,31 +7482,31 @@
         <v>40</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="X56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE56" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="Y56" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
@@ -7529,10 +7521,10 @@
         <v>42</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>361</v>
+        <v>42</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>274</v>
+        <v>364</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>42</v>
@@ -7540,7 +7532,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7563,18 +7555,16 @@
         <v>42</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>363</v>
+        <v>273</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="M57" s="2"/>
-      <c r="N57" t="s" s="2">
-        <v>366</v>
-      </c>
+      <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>42</v>
       </c>
@@ -7622,7 +7612,7 @@
         <v>42</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
@@ -7637,10 +7627,10 @@
         <v>42</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>42</v>
+        <v>345</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>42</v>
@@ -7648,7 +7638,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7659,7 +7649,7 @@
         <v>40</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>42</v>
@@ -7668,19 +7658,23 @@
         <v>42</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="O58" t="s" s="2">
         <v>42</v>
       </c>
@@ -7728,13 +7722,13 @@
         <v>42</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>42</v>
@@ -7743,10 +7737,10 @@
         <v>42</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>42</v>
@@ -7754,7 +7748,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7765,7 +7759,7 @@
         <v>40</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>42</v>
@@ -7774,23 +7768,19 @@
         <v>42</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>373</v>
+        <v>62</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>374</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>376</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>42</v>
       </c>
@@ -7838,13 +7828,13 @@
         <v>42</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>42</v>
@@ -7853,10 +7843,10 @@
         <v>42</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>377</v>
+        <v>42</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>378</v>
+        <v>64</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>42</v>
@@ -7864,18 +7854,18 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>42</v>
@@ -7887,15 +7877,17 @@
         <v>42</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="M60" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>42</v>
@@ -7944,13 +7936,13 @@
         <v>42</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>42</v>
@@ -7970,11 +7962,11 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -7987,7 +7979,7 @@
         <v>42</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I61" t="s" s="2">
         <v>42</v>
@@ -7996,10 +7988,10 @@
         <v>67</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>69</v>
+        <v>339</v>
       </c>
       <c r="M61" t="s" s="2">
         <v>70</v>
@@ -8052,7 +8044,7 @@
         <v>42</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8070,7 +8062,7 @@
         <v>42</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>42</v>
@@ -8078,47 +8070,49 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>341</v>
+        <v>42</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I62" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>171</v>
+        <v>380</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="N62" s="2"/>
+        <v>382</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>383</v>
+      </c>
       <c r="O62" t="s" s="2">
         <v>42</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" t="s" s="2">
-        <v>42</v>
+        <v>384</v>
       </c>
       <c r="R62" t="s" s="2">
         <v>42</v>
@@ -8136,13 +8130,13 @@
         <v>40</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>42</v>
+        <v>385</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>42</v>
+        <v>386</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>42</v>
@@ -8160,13 +8154,13 @@
         <v>42</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>42</v>
@@ -8175,10 +8169,10 @@
         <v>42</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>125</v>
+        <v>387</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>42</v>
@@ -8186,7 +8180,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8194,7 +8188,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F63" t="s" s="2">
         <v>51</v>
@@ -8209,26 +8203,22 @@
         <v>42</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>104</v>
+        <v>389</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>384</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="N63" t="s" s="2">
-        <v>386</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>42</v>
       </c>
       <c r="P63" s="2"/>
       <c r="Q63" t="s" s="2">
-        <v>387</v>
+        <v>42</v>
       </c>
       <c r="R63" t="s" s="2">
         <v>42</v>
@@ -8246,34 +8236,34 @@
         <v>40</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="X63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE63" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="Y63" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="Z63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE63" t="s" s="2">
-        <v>382</v>
-      </c>
       <c r="AF63" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>51</v>
@@ -8285,10 +8275,10 @@
         <v>42</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>42</v>
@@ -8296,7 +8286,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8304,10 +8294,10 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>42</v>
@@ -8316,19 +8306,23 @@
         <v>42</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>392</v>
+        <v>327</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
+        <v>395</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="N64" t="s" s="2">
+        <v>396</v>
+      </c>
       <c r="O64" t="s" s="2">
         <v>42</v>
       </c>
@@ -8376,13 +8370,13 @@
         <v>42</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>42</v>
@@ -8391,10 +8385,10 @@
         <v>42</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>42</v>
+        <v>397</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>42</v>
@@ -8402,7 +8396,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8422,23 +8416,19 @@
         <v>42</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>397</v>
+        <v>62</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>42</v>
       </c>
@@ -8486,13 +8476,13 @@
         <v>42</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>42</v>
@@ -8501,10 +8491,10 @@
         <v>42</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>400</v>
+        <v>42</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>401</v>
+        <v>64</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>42</v>
@@ -8512,18 +8502,18 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>42</v>
@@ -8535,15 +8525,17 @@
         <v>42</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="M66" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>42</v>
@@ -8592,13 +8584,13 @@
         <v>42</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>42</v>
@@ -8618,11 +8610,11 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
@@ -8635,7 +8627,7 @@
         <v>42</v>
       </c>
       <c r="H67" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I67" t="s" s="2">
         <v>42</v>
@@ -8644,10 +8636,10 @@
         <v>67</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>69</v>
+        <v>339</v>
       </c>
       <c r="M67" t="s" s="2">
         <v>70</v>
@@ -8700,7 +8692,7 @@
         <v>42</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>40</v>
@@ -8718,7 +8710,7 @@
         <v>42</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>42</v>
@@ -8726,41 +8718,41 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>341</v>
+        <v>42</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H68" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I68" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="I68" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="J68" t="s" s="2">
-        <v>67</v>
+        <v>156</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>171</v>
+        <v>403</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="N68" s="2"/>
+        <v>404</v>
+      </c>
+      <c r="M68" s="2"/>
+      <c r="N68" t="s" s="2">
+        <v>199</v>
+      </c>
       <c r="O68" t="s" s="2">
         <v>42</v>
       </c>
@@ -8784,13 +8776,13 @@
         <v>40</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>42</v>
+        <v>405</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>42</v>
+        <v>406</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>42</v>
@@ -8808,33 +8800,33 @@
         <v>42</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>42</v>
+        <v>407</v>
       </c>
       <c r="AI68" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>42</v>
+        <v>201</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>125</v>
+        <v>202</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>42</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8842,7 +8834,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F69" t="s" s="2">
         <v>51</v>
@@ -8857,17 +8849,19 @@
         <v>52</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>407</v>
-      </c>
-      <c r="M69" s="2"/>
+        <v>410</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>411</v>
+      </c>
       <c r="N69" t="s" s="2">
-        <v>202</v>
+        <v>251</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -8892,57 +8886,57 @@
         <v>40</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="X69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE69" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="Y69" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="AF69" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>51</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>410</v>
+        <v>42</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>204</v>
+        <v>253</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>205</v>
+        <v>254</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>206</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8962,22 +8956,22 @@
         <v>42</v>
       </c>
       <c r="I70" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>413</v>
+        <v>257</v>
       </c>
       <c r="M70" t="s" s="2">
         <v>414</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>42</v>
@@ -9002,13 +8996,11 @@
         <v>40</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>42</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="X70" s="2"/>
       <c r="Y70" t="s" s="2">
-        <v>42</v>
+        <v>260</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>42</v>
@@ -9026,7 +9018,7 @@
         <v>42</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9035,16 +9027,16 @@
         <v>51</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>42</v>
+        <v>261</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>256</v>
+        <v>125</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>42</v>
@@ -9063,7 +9055,7 @@
         <v>40</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>42</v>
@@ -9075,19 +9067,19 @@
         <v>42</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>156</v>
+        <v>327</v>
       </c>
       <c r="K71" t="s" s="2">
         <v>416</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>260</v>
+        <v>329</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>417</v>
+        <v>330</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>262</v>
+        <v>331</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>42</v>
@@ -9109,14 +9101,16 @@
         <v>42</v>
       </c>
       <c r="V71" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="W71" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="X71" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="Y71" t="s" s="2">
-        <v>263</v>
+        <v>42</v>
       </c>
       <c r="Z71" t="s" s="2">
         <v>42</v>
@@ -9140,19 +9134,19 @@
         <v>40</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>264</v>
+        <v>42</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>125</v>
+        <v>333</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>265</v>
+        <v>334</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>42</v>
@@ -9160,7 +9154,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9171,7 +9165,7 @@
         <v>40</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G72" t="s" s="2">
         <v>42</v>
@@ -9183,20 +9177,16 @@
         <v>42</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>419</v>
+        <v>62</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>334</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>42</v>
       </c>
@@ -9243,15 +9233,11 @@
       <c r="AD72" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="AE72" t="s" s="2">
-        <v>418</v>
-      </c>
+      <c r="AE72" s="2"/>
       <c r="AF72" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="AG72" t="s" s="2">
-        <v>41</v>
-      </c>
+      <c r="AG72" s="2"/>
       <c r="AH72" t="s" s="2">
         <v>42</v>
       </c>
@@ -9259,10 +9245,10 @@
         <v>42</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>336</v>
+        <v>42</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>337</v>
+        <v>64</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>42</v>
@@ -9270,18 +9256,18 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>42</v>
@@ -9293,15 +9279,17 @@
         <v>42</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="M73" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="M73" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
         <v>42</v>
@@ -9372,11 +9360,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9389,7 +9377,7 @@
         <v>42</v>
       </c>
       <c r="H74" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I74" t="s" s="2">
         <v>42</v>
@@ -9398,10 +9386,10 @@
         <v>67</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>69</v>
+        <v>339</v>
       </c>
       <c r="M74" t="s" s="2">
         <v>70</v>
@@ -9468,7 +9456,7 @@
         <v>42</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>42</v>
@@ -9476,40 +9464,38 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>341</v>
+        <v>42</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>42</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I75" t="s" s="2">
         <v>42</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>67</v>
+        <v>341</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>171</v>
+        <v>342</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>70</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
         <v>42</v>
@@ -9563,16 +9549,16 @@
       </c>
       <c r="AG75" s="2"/>
       <c r="AH75" t="s" s="2">
-        <v>42</v>
+        <v>344</v>
       </c>
       <c r="AI75" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ75" t="s" s="2">
-        <v>42</v>
+        <v>345</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>125</v>
+        <v>346</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>42</v>
@@ -9580,7 +9566,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9603,13 +9589,13 @@
         <v>42</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9665,16 +9651,16 @@
       </c>
       <c r="AG76" s="2"/>
       <c r="AH76" t="s" s="2">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AI76" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>42</v>
@@ -9682,7 +9668,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9705,16 +9691,20 @@
         <v>42</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>344</v>
+        <v>156</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="M77" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="N77" t="s" s="2">
+        <v>355</v>
+      </c>
       <c r="O77" t="s" s="2">
         <v>42</v>
       </c>
@@ -9738,13 +9728,13 @@
         <v>42</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>42</v>
+        <v>356</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>42</v>
+        <v>357</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>42</v>
@@ -9767,16 +9757,16 @@
       </c>
       <c r="AG77" s="2"/>
       <c r="AH77" t="s" s="2">
-        <v>347</v>
+        <v>42</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>353</v>
+        <v>271</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>42</v>
@@ -9784,7 +9774,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9807,19 +9797,17 @@
         <v>42</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>156</v>
+        <v>360</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>357</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="M78" s="2"/>
       <c r="N78" t="s" s="2">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="O78" t="s" s="2">
         <v>42</v>
@@ -9844,13 +9832,13 @@
         <v>42</v>
       </c>
       <c r="W78" t="s" s="2">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>359</v>
+        <v>42</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>360</v>
+        <v>42</v>
       </c>
       <c r="Z78" t="s" s="2">
         <v>42</v>
@@ -9879,10 +9867,10 @@
         <v>42</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>361</v>
+        <v>42</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>274</v>
+        <v>364</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>42</v>
@@ -9890,7 +9878,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9913,18 +9901,16 @@
         <v>42</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>363</v>
+        <v>273</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="M79" s="2"/>
-      <c r="N79" t="s" s="2">
-        <v>366</v>
-      </c>
+      <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>42</v>
       </c>
@@ -9983,119 +9969,17 @@
         <v>42</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>42</v>
+        <v>345</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="80" hidden="true">
-      <c r="A80" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F80" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="G80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="H80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="I80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="J80" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="K80" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="P80" s="2"/>
-      <c r="Q80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="R80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="S80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="T80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="U80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="V80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="W80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Y80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Z80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE80" s="2"/>
-      <c r="AF80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG80" s="2"/>
-      <c r="AH80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI80" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ80" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="AK80" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="AL80" t="s" s="2">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL80">
+  <autoFilter ref="A1:AL79">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10105,7 +9989,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI79">
+  <conditionalFormatting sqref="A2:AI78">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>